<commit_message>
Working on RESET issue
Send a GVER to receive the RCON register. After the RCON was send back it will be set to 0 (was written in the datasheet that we should do that).
</commit_message>
<xml_diff>
--- a/Documentation/ADC calculations.xlsx
+++ b/Documentation/ADC calculations.xlsx
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="N78" sqref="N78"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63:H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Working on the ADC issue
</commit_message>
<xml_diff>
--- a/Documentation/ADC calculations.xlsx
+++ b/Documentation/ADC calculations.xlsx
@@ -399,88 +399,88 @@
       <alignment horizontal="right" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63:H63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="S70" sqref="S70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -896,161 +896,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
@@ -1104,57 +1104,57 @@
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F17" s="2"/>
@@ -1261,26 +1261,26 @@
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="9"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="10">
+      <c r="K30" s="21">
         <v>42367</v>
       </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D31" s="3"/>
@@ -1296,21 +1296,21 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="9" t="s">
+      <c r="K32" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D33" s="3"/>
@@ -1326,624 +1326,624 @@
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="9" t="s">
+      <c r="K34" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25"/>
+      <c r="O43" s="25"/>
     </row>
     <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="25"/>
+      <c r="O44" s="25"/>
     </row>
     <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7" t="s">
+      <c r="B46" s="26"/>
+      <c r="C46" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7" t="s">
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7" t="s">
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="26"/>
+      <c r="N46" s="26"/>
+      <c r="O46" s="26"/>
     </row>
     <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="7"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="26"/>
+      <c r="N47" s="26"/>
+      <c r="O47" s="26"/>
     </row>
     <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="8">
+      <c r="B48" s="26"/>
+      <c r="C48" s="27">
         <v>42367</v>
       </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7" t="s">
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="7"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="26"/>
+      <c r="M48" s="26"/>
+      <c r="N48" s="26"/>
+      <c r="O48" s="26"/>
     </row>
     <row r="49" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="7"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="26"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="26"/>
     </row>
     <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="26"/>
+      <c r="M50" s="26"/>
+      <c r="N50" s="26"/>
+      <c r="O50" s="26"/>
     </row>
     <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="26"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="26"/>
     </row>
     <row r="52" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7"/>
-      <c r="O52" s="7"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="26"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
     </row>
     <row r="55" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17" t="s">
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17" t="s">
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17" t="s">
+      <c r="J55" s="19"/>
+      <c r="K55" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="L55" s="17"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="17"/>
+      <c r="L55" s="19"/>
+      <c r="M55" s="19"/>
+      <c r="N55" s="19"/>
     </row>
     <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="19"/>
+      <c r="N56" s="19"/>
     </row>
     <row r="57" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="16">
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="11">
         <v>80000000</v>
       </c>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
-      <c r="I57" s="16" t="s">
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J57" s="16"/>
-      <c r="K57" s="15" t="s">
+      <c r="J57" s="11"/>
+      <c r="K57" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="L57" s="15"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="15"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
     </row>
     <row r="58" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="16">
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="11">
         <v>1</v>
       </c>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16" t="s">
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J58" s="16"/>
-      <c r="K58" s="15" t="s">
+      <c r="J58" s="11"/>
+      <c r="K58" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L58" s="15"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
     </row>
     <row r="59" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="21">
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="10">
         <f>F57/F58</f>
         <v>80000000</v>
       </c>
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="16" t="s">
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J59" s="16"/>
-      <c r="K59" s="15" t="s">
+      <c r="J59" s="11"/>
+      <c r="K59" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L59" s="15"/>
-      <c r="M59" s="15"/>
-      <c r="N59" s="15"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
     </row>
     <row r="60" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="22">
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="18">
         <f>1/F59</f>
         <v>1.2499999999999999E-8</v>
       </c>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
-      <c r="I60" s="16" t="s">
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J60" s="16"/>
-      <c r="K60" s="15" t="s">
+      <c r="J60" s="11"/>
+      <c r="K60" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
     </row>
     <row r="61" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="18"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="19"/>
-      <c r="M61" s="19"/>
-      <c r="N61" s="20"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="16"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="17"/>
     </row>
     <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="16">
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="11">
         <v>10</v>
       </c>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16"/>
-      <c r="I62" s="16" t="s">
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J62" s="16"/>
-      <c r="K62" s="15" t="s">
+      <c r="J62" s="11"/>
+      <c r="K62" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L62" s="15"/>
-      <c r="M62" s="15"/>
-      <c r="N62" s="15"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
     </row>
     <row r="63" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="21">
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="10">
         <f>2*(F60*(F62+1))</f>
         <v>2.7500000000000001E-7</v>
       </c>
-      <c r="G63" s="21"/>
-      <c r="H63" s="21"/>
-      <c r="I63" s="16" t="s">
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J63" s="16"/>
-      <c r="K63" s="15" t="s">
+      <c r="J63" s="11"/>
+      <c r="K63" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="L63" s="15"/>
-      <c r="M63" s="15"/>
-      <c r="N63" s="15"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="9"/>
     </row>
     <row r="64" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15"/>
-      <c r="F64" s="16">
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="11">
         <v>2</v>
       </c>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="16" t="s">
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J64" s="16"/>
-      <c r="K64" s="15" t="s">
+      <c r="J64" s="11"/>
+      <c r="K64" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L64" s="15"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="15"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
     </row>
     <row r="65" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="18"/>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
-      <c r="J65" s="19"/>
-      <c r="K65" s="19"/>
-      <c r="L65" s="19"/>
-      <c r="M65" s="19"/>
-      <c r="N65" s="20"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="16"/>
+      <c r="M65" s="16"/>
+      <c r="N65" s="17"/>
     </row>
     <row r="66" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="15" t="s">
+      <c r="B66" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="21">
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="10">
         <f>F64*F63</f>
         <v>5.5000000000000003E-7</v>
       </c>
-      <c r="G66" s="21"/>
-      <c r="H66" s="21"/>
-      <c r="I66" s="16" t="s">
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J66" s="16"/>
-      <c r="K66" s="15" t="s">
+      <c r="J66" s="11"/>
+      <c r="K66" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="L66" s="15"/>
-      <c r="M66" s="15"/>
-      <c r="N66" s="15"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="9"/>
     </row>
     <row r="67" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="21">
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="10">
         <f>12*F63</f>
         <v>3.3000000000000002E-6</v>
       </c>
-      <c r="G67" s="21"/>
-      <c r="H67" s="21"/>
-      <c r="I67" s="16" t="s">
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J67" s="16"/>
-      <c r="K67" s="15" t="s">
+      <c r="J67" s="11"/>
+      <c r="K67" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="L67" s="15"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="15"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
     </row>
     <row r="68" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="15"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
-      <c r="I68" s="16"/>
-      <c r="J68" s="16"/>
-      <c r="K68" s="15"/>
-      <c r="L68" s="15"/>
-      <c r="M68" s="15"/>
-      <c r="N68" s="15"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
     </row>
     <row r="69" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="21">
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="10">
         <f>F66+F67</f>
         <v>3.8500000000000004E-6</v>
       </c>
-      <c r="G69" s="21"/>
-      <c r="H69" s="21"/>
-      <c r="I69" s="16" t="s">
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J69" s="16"/>
-      <c r="K69" s="15" t="s">
+      <c r="J69" s="11"/>
+      <c r="K69" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L69" s="15"/>
-      <c r="M69" s="15"/>
-      <c r="N69" s="15"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
     </row>
     <row r="70" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="25" t="s">
+      <c r="B70" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="26">
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="13">
         <f>(1/F69)/1000</f>
         <v>259.74025974025972</v>
       </c>
-      <c r="G70" s="26"/>
-      <c r="H70" s="26"/>
-      <c r="I70" s="27" t="s">
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J70" s="27"/>
-      <c r="K70" s="23"/>
-      <c r="L70" s="23"/>
-      <c r="M70" s="23"/>
-      <c r="N70" s="23"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="7"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+      <c r="N70" s="7"/>
     </row>
     <row r="71" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="23"/>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="24"/>
-      <c r="J71" s="24"/>
-      <c r="K71" s="23"/>
-      <c r="L71" s="23"/>
-      <c r="M71" s="23"/>
-      <c r="N71" s="23"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="8"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7"/>
     </row>
     <row r="72" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="23"/>
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="24"/>
-      <c r="H72" s="24"/>
-      <c r="I72" s="24"/>
-      <c r="J72" s="24"/>
-      <c r="K72" s="23"/>
-      <c r="L72" s="23"/>
-      <c r="M72" s="23"/>
-      <c r="N72" s="23"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
     </row>
     <row r="73" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="23"/>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="24"/>
-      <c r="H73" s="24"/>
-      <c r="I73" s="24"/>
-      <c r="J73" s="24"/>
-      <c r="K73" s="23"/>
-      <c r="L73" s="23"/>
-      <c r="M73" s="23"/>
-      <c r="N73" s="23"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
+      <c r="N73" s="7"/>
     </row>
     <row r="74" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="23"/>
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="24"/>
-      <c r="H74" s="24"/>
-      <c r="I74" s="24"/>
-      <c r="J74" s="24"/>
-      <c r="K74" s="23"/>
-      <c r="L74" s="23"/>
-      <c r="M74" s="23"/>
-      <c r="N74" s="23"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="7"/>
+      <c r="N74" s="7"/>
     </row>
     <row r="75" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="23"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
-      <c r="E75" s="23"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="24"/>
-      <c r="H75" s="24"/>
-      <c r="I75" s="24"/>
-      <c r="J75" s="24"/>
-      <c r="K75" s="23"/>
-      <c r="L75" s="23"/>
-      <c r="M75" s="23"/>
-      <c r="N75" s="23"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="8"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="7"/>
+      <c r="N75" s="7"/>
     </row>
     <row r="76" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="23"/>
-      <c r="C76" s="23"/>
-      <c r="D76" s="23"/>
-      <c r="E76" s="23"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="24"/>
-      <c r="H76" s="24"/>
-      <c r="I76" s="24"/>
-      <c r="J76" s="24"/>
-      <c r="K76" s="23"/>
-      <c r="L76" s="23"/>
-      <c r="M76" s="23"/>
-      <c r="N76" s="23"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="8"/>
+      <c r="K76" s="7"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
+      <c r="N76" s="7"/>
     </row>
     <row r="1048576" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I1048576" s="2"/>
@@ -1956,100 +1956,6 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:N75"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="K76:N76"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="K73:N73"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:N71"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K72:N72"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="K69:N69"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:N70"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="K67:N67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="K68:N68"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:N66"/>
-    <mergeCell ref="B65:N65"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="K63:N63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="K64:N64"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="I62:J62"/>
-    <mergeCell ref="K62:N62"/>
-    <mergeCell ref="B61:N61"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:N59"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="K60:N60"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:N57"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:N58"/>
-    <mergeCell ref="B55:E56"/>
-    <mergeCell ref="F55:H56"/>
-    <mergeCell ref="I55:J56"/>
-    <mergeCell ref="K55:N56"/>
-    <mergeCell ref="D30:I30"/>
-    <mergeCell ref="K30:N30"/>
-    <mergeCell ref="A1:O3"/>
-    <mergeCell ref="A4:O6"/>
-    <mergeCell ref="A7:O9"/>
-    <mergeCell ref="A13:O15"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A43:O44"/>
-    <mergeCell ref="J46:O47"/>
-    <mergeCell ref="F46:I47"/>
-    <mergeCell ref="C46:E47"/>
-    <mergeCell ref="A46:B47"/>
-    <mergeCell ref="D32:I32"/>
-    <mergeCell ref="D34:I34"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="K34:N34"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="F48:I48"/>
@@ -2070,6 +1976,100 @@
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="F51:I51"/>
     <mergeCell ref="J51:O51"/>
+    <mergeCell ref="D30:I30"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="A1:O3"/>
+    <mergeCell ref="A4:O6"/>
+    <mergeCell ref="A7:O9"/>
+    <mergeCell ref="A13:O15"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A43:O44"/>
+    <mergeCell ref="J46:O47"/>
+    <mergeCell ref="F46:I47"/>
+    <mergeCell ref="C46:E47"/>
+    <mergeCell ref="A46:B47"/>
+    <mergeCell ref="D32:I32"/>
+    <mergeCell ref="D34:I34"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:N57"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:N58"/>
+    <mergeCell ref="B55:E56"/>
+    <mergeCell ref="F55:H56"/>
+    <mergeCell ref="I55:J56"/>
+    <mergeCell ref="K55:N56"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="K62:N62"/>
+    <mergeCell ref="B61:N61"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:N59"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="K60:N60"/>
+    <mergeCell ref="B65:N65"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="K63:N63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="K64:N64"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="K67:N67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="K68:N68"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:N66"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:N71"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:N72"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="K69:N69"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:N70"/>
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="K73:N73"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="K74:N74"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.98" right="0.79000000000000015" top="1.57" bottom="1.18" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Worked on the ADC calculation.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/ADC calculations.xlsx
+++ b/Documentation/ADC calculations.xlsx
@@ -399,6 +399,70 @@
       <alignment horizontal="right" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -407,18 +471,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -429,58 +481,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="S70" sqref="S70"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65:N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -896,161 +896,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
@@ -1104,57 +1104,57 @@
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F17" s="2"/>
@@ -1261,26 +1261,26 @@
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="20"/>
+      <c r="B30" s="9"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="21">
+      <c r="K30" s="10">
         <v>42367</v>
       </c>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D31" s="3"/>
@@ -1296,21 +1296,21 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="20" t="s">
+      <c r="K32" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D33" s="3"/>
@@ -1326,624 +1326,624 @@
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="20" t="s">
+      <c r="K34" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="25"/>
-      <c r="O43" s="25"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
     </row>
     <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
-      <c r="L44" s="25"/>
-      <c r="M44" s="25"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="25"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
     </row>
     <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26" t="s">
+      <c r="B46" s="7"/>
+      <c r="C46" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26" t="s">
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26" t="s">
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K46" s="26"/>
-      <c r="L46" s="26"/>
-      <c r="M46" s="26"/>
-      <c r="N46" s="26"/>
-      <c r="O46" s="26"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
     </row>
     <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="26"/>
-      <c r="L47" s="26"/>
-      <c r="M47" s="26"/>
-      <c r="N47" s="26"/>
-      <c r="O47" s="26"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
     </row>
     <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="27">
+      <c r="B48" s="7"/>
+      <c r="C48" s="8">
         <v>42367</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26" t="s">
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26" t="s">
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K48" s="26"/>
-      <c r="L48" s="26"/>
-      <c r="M48" s="26"/>
-      <c r="N48" s="26"/>
-      <c r="O48" s="26"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
     </row>
     <row r="49" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="26"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="26"/>
-      <c r="O49" s="26"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
     </row>
     <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="26"/>
-      <c r="K50" s="26"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="26"/>
-      <c r="N50" s="26"/>
-      <c r="O50" s="26"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
     </row>
     <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="26"/>
-      <c r="M51" s="26"/>
-      <c r="N51" s="26"/>
-      <c r="O51" s="26"/>
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
     </row>
     <row r="52" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="26"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="26"/>
-      <c r="J52" s="26"/>
-      <c r="K52" s="26"/>
-      <c r="L52" s="26"/>
-      <c r="M52" s="26"/>
-      <c r="N52" s="26"/>
-      <c r="O52" s="26"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7"/>
     </row>
     <row r="55" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="19" t="s">
+      <c r="B55" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19" t="s">
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19" t="s">
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19" t="s">
+      <c r="J55" s="17"/>
+      <c r="K55" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L55" s="19"/>
-      <c r="M55" s="19"/>
-      <c r="N55" s="19"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
     </row>
     <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="19"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="19"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="19"/>
-      <c r="M56" s="19"/>
-      <c r="N56" s="19"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
     </row>
     <row r="57" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="11">
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="16">
         <v>80000000</v>
       </c>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11" t="s">
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J57" s="11"/>
-      <c r="K57" s="9" t="s">
+      <c r="J57" s="16"/>
+      <c r="K57" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L57" s="9"/>
-      <c r="M57" s="9"/>
-      <c r="N57" s="9"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
     </row>
     <row r="58" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="11">
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="16">
         <v>1</v>
       </c>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11" t="s">
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J58" s="11"/>
-      <c r="K58" s="9" t="s">
+      <c r="J58" s="16"/>
+      <c r="K58" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="L58" s="9"/>
-      <c r="M58" s="9"/>
-      <c r="N58" s="9"/>
+      <c r="L58" s="15"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15"/>
     </row>
     <row r="59" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="10">
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="21">
         <f>F57/F58</f>
         <v>80000000</v>
       </c>
-      <c r="G59" s="10"/>
-      <c r="H59" s="10"/>
-      <c r="I59" s="11" t="s">
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J59" s="11"/>
-      <c r="K59" s="9" t="s">
+      <c r="J59" s="16"/>
+      <c r="K59" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
-      <c r="N59" s="9"/>
+      <c r="L59" s="15"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15"/>
     </row>
     <row r="60" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="18">
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="22">
         <f>1/F59</f>
         <v>1.2499999999999999E-8</v>
       </c>
-      <c r="G60" s="18"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="11" t="s">
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J60" s="11"/>
-      <c r="K60" s="9" t="s">
+      <c r="J60" s="16"/>
+      <c r="K60" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="L60" s="9"/>
-      <c r="M60" s="9"/>
-      <c r="N60" s="9"/>
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15"/>
     </row>
     <row r="61" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="15"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="16"/>
-      <c r="J61" s="16"/>
-      <c r="K61" s="16"/>
-      <c r="L61" s="16"/>
-      <c r="M61" s="16"/>
-      <c r="N61" s="17"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="19"/>
+      <c r="M61" s="19"/>
+      <c r="N61" s="20"/>
     </row>
     <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="11">
-        <v>10</v>
-      </c>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11" t="s">
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="16">
+        <v>40</v>
+      </c>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J62" s="11"/>
-      <c r="K62" s="9" t="s">
+      <c r="J62" s="16"/>
+      <c r="K62" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
-      <c r="N62" s="9"/>
+      <c r="L62" s="15"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15"/>
     </row>
     <row r="63" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="10">
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="21">
         <f>2*(F60*(F62+1))</f>
-        <v>2.7500000000000001E-7</v>
-      </c>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="11" t="s">
+        <v>1.0249999999999999E-6</v>
+      </c>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J63" s="11"/>
-      <c r="K63" s="9" t="s">
+      <c r="J63" s="16"/>
+      <c r="K63" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="L63" s="9"/>
-      <c r="M63" s="9"/>
-      <c r="N63" s="9"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
     </row>
     <row r="64" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="11">
-        <v>2</v>
-      </c>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11" t="s">
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="16">
+        <v>31</v>
+      </c>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J64" s="11"/>
-      <c r="K64" s="9" t="s">
+      <c r="J64" s="16"/>
+      <c r="K64" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="L64" s="9"/>
-      <c r="M64" s="9"/>
-      <c r="N64" s="9"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
     </row>
     <row r="65" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="15"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
-      <c r="J65" s="16"/>
-      <c r="K65" s="16"/>
-      <c r="L65" s="16"/>
-      <c r="M65" s="16"/>
-      <c r="N65" s="17"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="19"/>
+      <c r="L65" s="19"/>
+      <c r="M65" s="19"/>
+      <c r="N65" s="20"/>
     </row>
     <row r="66" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="10">
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="21">
         <f>F64*F63</f>
-        <v>5.5000000000000003E-7</v>
-      </c>
-      <c r="G66" s="10"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="11" t="s">
+        <v>3.1775E-5</v>
+      </c>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J66" s="11"/>
-      <c r="K66" s="9" t="s">
+      <c r="J66" s="16"/>
+      <c r="K66" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="L66" s="9"/>
-      <c r="M66" s="9"/>
-      <c r="N66" s="9"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
     </row>
     <row r="67" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="10">
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="21">
         <f>12*F63</f>
-        <v>3.3000000000000002E-6</v>
-      </c>
-      <c r="G67" s="10"/>
-      <c r="H67" s="10"/>
-      <c r="I67" s="11" t="s">
+        <v>1.2299999999999999E-5</v>
+      </c>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J67" s="11"/>
-      <c r="K67" s="9" t="s">
+      <c r="J67" s="16"/>
+      <c r="K67" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="L67" s="9"/>
-      <c r="M67" s="9"/>
-      <c r="N67" s="9"/>
+      <c r="L67" s="15"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
     </row>
     <row r="68" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="9"/>
-      <c r="L68" s="9"/>
-      <c r="M68" s="9"/>
-      <c r="N68" s="9"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="16"/>
+      <c r="J68" s="16"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="15"/>
     </row>
     <row r="69" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="10">
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="21">
         <f>F66+F67</f>
-        <v>3.8500000000000004E-6</v>
-      </c>
-      <c r="G69" s="10"/>
-      <c r="H69" s="10"/>
-      <c r="I69" s="11" t="s">
+        <v>4.4075000000000001E-5</v>
+      </c>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J69" s="11"/>
-      <c r="K69" s="9" t="s">
+      <c r="J69" s="16"/>
+      <c r="K69" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="L69" s="9"/>
-      <c r="M69" s="9"/>
-      <c r="N69" s="9"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
     </row>
     <row r="70" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="12" t="s">
+      <c r="B70" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="13">
+      <c r="C70" s="25"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="26">
         <f>(1/F69)/1000</f>
-        <v>259.74025974025972</v>
-      </c>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="14" t="s">
+        <v>22.688598979013044</v>
+      </c>
+      <c r="G70" s="26"/>
+      <c r="H70" s="26"/>
+      <c r="I70" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J70" s="14"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="7"/>
-      <c r="M70" s="7"/>
-      <c r="N70" s="7"/>
+      <c r="J70" s="27"/>
+      <c r="K70" s="23"/>
+      <c r="L70" s="23"/>
+      <c r="M70" s="23"/>
+      <c r="N70" s="23"/>
     </row>
     <row r="71" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
-      <c r="J71" s="8"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="7"/>
-      <c r="M71" s="7"/>
-      <c r="N71" s="7"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="24"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="24"/>
+      <c r="J71" s="24"/>
+      <c r="K71" s="23"/>
+      <c r="L71" s="23"/>
+      <c r="M71" s="23"/>
+      <c r="N71" s="23"/>
     </row>
     <row r="72" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="8"/>
-      <c r="I72" s="8"/>
-      <c r="J72" s="8"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7"/>
-      <c r="N72" s="7"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="24"/>
+      <c r="J72" s="24"/>
+      <c r="K72" s="23"/>
+      <c r="L72" s="23"/>
+      <c r="M72" s="23"/>
+      <c r="N72" s="23"/>
     </row>
     <row r="73" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
-      <c r="I73" s="8"/>
-      <c r="J73" s="8"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
-      <c r="N73" s="7"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="24"/>
+      <c r="J73" s="24"/>
+      <c r="K73" s="23"/>
+      <c r="L73" s="23"/>
+      <c r="M73" s="23"/>
+      <c r="N73" s="23"/>
     </row>
     <row r="74" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="8"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="7"/>
-      <c r="L74" s="7"/>
-      <c r="M74" s="7"/>
-      <c r="N74" s="7"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="24"/>
+      <c r="I74" s="24"/>
+      <c r="J74" s="24"/>
+      <c r="K74" s="23"/>
+      <c r="L74" s="23"/>
+      <c r="M74" s="23"/>
+      <c r="N74" s="23"/>
     </row>
     <row r="75" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
-      <c r="J75" s="8"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="7"/>
-      <c r="M75" s="7"/>
-      <c r="N75" s="7"/>
+      <c r="B75" s="23"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="24"/>
+      <c r="I75" s="24"/>
+      <c r="J75" s="24"/>
+      <c r="K75" s="23"/>
+      <c r="L75" s="23"/>
+      <c r="M75" s="23"/>
+      <c r="N75" s="23"/>
     </row>
     <row r="76" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="8"/>
-      <c r="G76" s="8"/>
-      <c r="H76" s="8"/>
-      <c r="I76" s="8"/>
-      <c r="J76" s="8"/>
-      <c r="K76" s="7"/>
-      <c r="L76" s="7"/>
-      <c r="M76" s="7"/>
-      <c r="N76" s="7"/>
+      <c r="B76" s="23"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="24"/>
+      <c r="H76" s="24"/>
+      <c r="I76" s="24"/>
+      <c r="J76" s="24"/>
+      <c r="K76" s="23"/>
+      <c r="L76" s="23"/>
+      <c r="M76" s="23"/>
+      <c r="N76" s="23"/>
     </row>
     <row r="1048576" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I1048576" s="2"/>
@@ -1956,6 +1956,100 @@
     </row>
   </sheetData>
   <mergeCells count="114">
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="K73:N73"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:N71"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:N72"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="K69:N69"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:N70"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="K67:N67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="K68:N68"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:N66"/>
+    <mergeCell ref="B65:N65"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="K63:N63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="K64:N64"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="K62:N62"/>
+    <mergeCell ref="B61:N61"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:N59"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="K60:N60"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:N57"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:N58"/>
+    <mergeCell ref="B55:E56"/>
+    <mergeCell ref="F55:H56"/>
+    <mergeCell ref="I55:J56"/>
+    <mergeCell ref="K55:N56"/>
+    <mergeCell ref="D30:I30"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="A1:O3"/>
+    <mergeCell ref="A4:O6"/>
+    <mergeCell ref="A7:O9"/>
+    <mergeCell ref="A13:O15"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A43:O44"/>
+    <mergeCell ref="J46:O47"/>
+    <mergeCell ref="F46:I47"/>
+    <mergeCell ref="C46:E47"/>
+    <mergeCell ref="A46:B47"/>
+    <mergeCell ref="D32:I32"/>
+    <mergeCell ref="D34:I34"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="K34:N34"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="F48:I48"/>
@@ -1976,100 +2070,6 @@
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="F51:I51"/>
     <mergeCell ref="J51:O51"/>
-    <mergeCell ref="D30:I30"/>
-    <mergeCell ref="K30:N30"/>
-    <mergeCell ref="A1:O3"/>
-    <mergeCell ref="A4:O6"/>
-    <mergeCell ref="A7:O9"/>
-    <mergeCell ref="A13:O15"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A43:O44"/>
-    <mergeCell ref="J46:O47"/>
-    <mergeCell ref="F46:I47"/>
-    <mergeCell ref="C46:E47"/>
-    <mergeCell ref="A46:B47"/>
-    <mergeCell ref="D32:I32"/>
-    <mergeCell ref="D34:I34"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:N57"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:N58"/>
-    <mergeCell ref="B55:E56"/>
-    <mergeCell ref="F55:H56"/>
-    <mergeCell ref="I55:J56"/>
-    <mergeCell ref="K55:N56"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="I62:J62"/>
-    <mergeCell ref="K62:N62"/>
-    <mergeCell ref="B61:N61"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:N59"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="K60:N60"/>
-    <mergeCell ref="B65:N65"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="K63:N63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="K64:N64"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="K67:N67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="K68:N68"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:N66"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:N71"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K72:N72"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="K69:N69"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:N70"/>
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:N75"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="K76:N76"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="K73:N73"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="K74:N74"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.98" right="0.79000000000000015" top="1.57" bottom="1.18" header="0.5" footer="0.5"/>

</xml_diff>